<commit_message>
P1 Done with a few bugs
</commit_message>
<xml_diff>
--- a/Projects/Project 1/ProjectDetha/ExcelSheets/Expenses.xlsx
+++ b/Projects/Project 1/ProjectDetha/ExcelSheets/Expenses.xlsx
@@ -1,56 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:workbookPr codeName="ThisWorkbook"/>
+  <x:bookViews>
+    <x:workbookView firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="125725"/>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-</styleSheet>
+<x:styleSheet xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </x:numFmts>
+  <x:fonts count="2">
+    <x:font>
+      <x:sz val="12"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,26 +406,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>id</v>
-      </c>
-      <c r="B1" t="str">
-        <v>customerId</v>
-      </c>
-      <c r="C1" t="str">
-        <v>TotalAmount</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C1"/>
-  </ignoredErrors>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B4" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:ignoredErrors>
+    <x:ignoredError sqref="A1:C1" numberStoredAsText="1"/>
+  </x:ignoredErrors>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>